<commit_message>
AUD New Framework + JPY bug fix
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD/AUD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD/AUD_YCSTDBootstrapping.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="GeneralSettings" sheetId="1" r:id="rId1"/>
-    <sheet name="EURSTD" sheetId="15" r:id="rId2"/>
+    <sheet name="AUDSTD" sheetId="15" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -19,15 +19,15 @@
     <definedName name="Discounting">GeneralSettings!$D$7</definedName>
     <definedName name="Evaluationdate">GeneralSettings!$D$12</definedName>
     <definedName name="FamilyName">GeneralSettings!$D$8</definedName>
-    <definedName name="IncludeFlag" localSheetId="1">EURSTD!$P$3:$P$110</definedName>
-    <definedName name="MinDistance" localSheetId="1">EURSTD!$R$3:$R$110</definedName>
+    <definedName name="IncludeFlag" localSheetId="1">AUDSTD!$P$3:$P$110</definedName>
+    <definedName name="MinDistance" localSheetId="1">AUDSTD!$R$3:$R$110</definedName>
     <definedName name="ObjectOverwrite">GeneralSettings!$D$6</definedName>
     <definedName name="Permanent">GeneralSettings!$D$4</definedName>
     <definedName name="PillarDate">GeneralSettings!$D$10</definedName>
-    <definedName name="Priority" localSheetId="1">EURSTD!$Q$3:$Q$110</definedName>
+    <definedName name="Priority" localSheetId="1">AUDSTD!$Q$3:$Q$110</definedName>
     <definedName name="QuoteSuffix">GeneralSettings!$D$9</definedName>
-    <definedName name="RateHelpers" localSheetId="1">EURSTD!$M$3:$M$110</definedName>
-    <definedName name="RateHelpersSTD">EURSTD!$W$3:$W$110</definedName>
+    <definedName name="RateHelpers" localSheetId="1">AUDSTD!$M$3:$M$110</definedName>
+    <definedName name="RateHelpersSTD">AUDSTD!$W$3:$W$110</definedName>
     <definedName name="Settlementdate">GeneralSettings!$D$13</definedName>
     <definedName name="Trigger">GeneralSettings!$D$5</definedName>
     <definedName name="YieldCurve_STD">GeneralSettings!$D$18</definedName>
@@ -1315,8 +1315,8 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="13">
-          <cell r="J13" t="str">
+        <row r="11">
+          <cell r="J11" t="str">
             <v>AUDSTD#0000</v>
           </cell>
         </row>
@@ -1678,9 +1678,7 @@
       <c r="C5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="21">
-        <v>42272.583819444444</v>
-      </c>
+      <c r="D5" s="21"/>
       <c r="E5" s="80"/>
     </row>
     <row r="6" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1747,7 +1745,7 @@
       </c>
       <c r="D12" s="13">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="E12" s="80"/>
     </row>
@@ -1758,7 +1756,7 @@
       </c>
       <c r="D13" s="15">
         <f>_xll.qlCalendarAdvance(Calendar,Evaluationdate,"1D","F",,Trigger)</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="E13" s="80"/>
     </row>
@@ -1869,7 +1867,7 @@
       <c r="B26" s="23"/>
       <c r="C26" s="32">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve_STD)</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="D26" s="33">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C26,,Trigger)</f>
@@ -1882,18 +1880,18 @@
       <c r="B27" s="23"/>
       <c r="C27" s="34">
         <f>_xll.qlTermStructureMaxDate(YieldCurve_STD,Trigger)</f>
-        <v>53146</v>
+        <v>53245</v>
       </c>
       <c r="D27" s="35">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C27,,Trigger)</f>
-        <v>0.30965633738822224</v>
+        <v>0.36667594533189724</v>
       </c>
       <c r="E27" s="42"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B28" s="23"/>
       <c r="C28" s="34" t="str">
-        <f>[1]BBSW!$J$13</f>
+        <f>[1]BBSW!$J$11</f>
         <v>AUDSTD#0000</v>
       </c>
       <c r="D28" s="35" t="b">
@@ -1908,7 +1906,8 @@
         <v>99</v>
       </c>
       <c r="D29" s="37" t="b">
-        <v>0</v>
+        <f>_xll.qlExtrapolatorEnableExtrapolation(YieldCurve_STD,TRUE,Trigger)</f>
+        <v>1</v>
       </c>
       <c r="E29" s="42"/>
     </row>
@@ -1953,7 +1952,7 @@
   <dimension ref="A1:AH127"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2103,7 +2102,7 @@
       </c>
       <c r="AC2" s="155">
         <f t="array" ref="AC2:AC110">_xll.qlPiecewiseYieldCurveData(YieldCurve_STD,Trigger)</f>
-        <v>2.2497919777007814E-2</v>
+        <v>2.2997101856854614E-2</v>
       </c>
       <c r="AD2" s="158"/>
       <c r="AE2" s="163" t="s">
@@ -2135,7 +2134,7 @@
       <c r="I3" s="120"/>
       <c r="J3" s="110" t="str">
         <f>_xll.qlDepositRateHelper(,H3,G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00263#0000</v>
+        <v>obj_002a9#0002</v>
       </c>
       <c r="K3" s="49"/>
       <c r="L3" s="66" t="str">
@@ -2144,15 +2143,15 @@
       </c>
       <c r="M3" s="128" t="str">
         <f>IF(ISBLANK(J3),"--",J3)</f>
-        <v>obj_00263#0000</v>
+        <v>obj_002a9#0002</v>
       </c>
       <c r="N3" s="142" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M3,Trigger),"--")</f>
         <v>AUDOND_Quote</v>
       </c>
-      <c r="O3" s="130">
+      <c r="O3" s="130" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M3,Trigger),"--")</f>
-        <v>0.02</v>
+        <v>--</v>
       </c>
       <c r="P3" s="129" t="b">
         <v>0</v>
@@ -2165,11 +2164,11 @@
       </c>
       <c r="S3" s="131">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M3,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T3" s="131">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M3,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="U3" s="159"/>
       <c r="V3" s="3" t="str">
@@ -2178,7 +2177,7 @@
       </c>
       <c r="W3" s="3" t="str">
         <f t="array" ref="W3:W110">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,IncludeFlag),_xll.ohFilter(Priority,IncludeFlag),$AF$3,$AF$4,$AF$5,$AF$6,_xll.ohFilter(MinDistance,IncludeFlag),Trigger)</f>
-        <v>obj_00260</v>
+        <v>obj_002a5</v>
       </c>
       <c r="X3" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W3,Trigger),"")</f>
@@ -2186,7 +2185,7 @@
       </c>
       <c r="Y3" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W3,Trigger),"")</f>
-        <v>2.2499999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="Z3" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W3)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W3)),_xll.qlSwapRateHelperSpread($W3))</f>
@@ -2194,14 +2193,14 @@
       </c>
       <c r="AA3" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W3,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB3" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W3,Trigger),"")</f>
-        <v>42184</v>
+        <v>42283</v>
       </c>
       <c r="AC3" s="68">
-        <v>2.2497919777007814E-2</v>
+        <v>2.2997101856854614E-2</v>
       </c>
       <c r="AD3" s="158"/>
       <c r="AE3" s="103" t="s">
@@ -2235,7 +2234,7 @@
       <c r="I4" s="127"/>
       <c r="J4" s="57" t="str">
         <f>_xll.qlFraRateHelper(,H4,"1D",G4,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00260#0000</v>
+        <v>obj_002a5#0002</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="9" t="str">
@@ -2244,7 +2243,7 @@
       </c>
       <c r="M4" s="90" t="str">
         <f t="shared" ref="M4:M14" si="2">IF(ISBLANK(J4),"--",J4)</f>
-        <v>obj_00260#0000</v>
+        <v>obj_002a5#0002</v>
       </c>
       <c r="N4" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M4,Trigger),"--")</f>
@@ -2252,7 +2251,7 @@
       </c>
       <c r="O4" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M4,Trigger),"--")</f>
-        <v>2.2499999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="P4" s="93" t="b">
         <v>1</v>
@@ -2265,11 +2264,11 @@
       </c>
       <c r="S4" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M4,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T4" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M4,Trigger),"--")</f>
-        <v>42184</v>
+        <v>42283</v>
       </c>
       <c r="U4" s="159"/>
       <c r="V4" s="3" t="str">
@@ -2277,7 +2276,7 @@
         <v>Dp</v>
       </c>
       <c r="W4" s="3" t="str">
-        <v>obj_00250</v>
+        <v>obj_00290</v>
       </c>
       <c r="X4" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W4,Trigger),"")</f>
@@ -2285,7 +2284,7 @@
       </c>
       <c r="Y4" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W4,Trigger),"")</f>
-        <v>2.2499999999999999E-2</v>
+        <v>2.0750000000000001E-2</v>
       </c>
       <c r="Z4" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W4)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W4)),_xll.qlSwapRateHelperSpread($W4))</f>
@@ -2293,14 +2292,14 @@
       </c>
       <c r="AA4" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W4,Trigger),"")</f>
-        <v>42184</v>
+        <v>42283</v>
       </c>
       <c r="AB4" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W4,Trigger),"")</f>
-        <v>42185</v>
+        <v>42284</v>
       </c>
       <c r="AC4" s="68">
-        <v>2.2498197128676015E-2</v>
+        <v>2.2622486582502554E-2</v>
       </c>
       <c r="AD4" s="158"/>
       <c r="AE4" s="103" t="s">
@@ -2334,7 +2333,7 @@
       <c r="I5" s="122"/>
       <c r="J5" s="2" t="str">
         <f>_xll.qlFraRateHelper(,H5,"2D",G5,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00250#0000</v>
+        <v>obj_00290#0002</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="9" t="str">
@@ -2343,7 +2342,7 @@
       </c>
       <c r="M5" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_00250#0000</v>
+        <v>obj_00290#0002</v>
       </c>
       <c r="N5" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M5,Trigger),"--")</f>
@@ -2351,7 +2350,7 @@
       </c>
       <c r="O5" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M5,Trigger),"--")</f>
-        <v>2.2499999999999999E-2</v>
+        <v>2.0750000000000001E-2</v>
       </c>
       <c r="P5" s="93" t="b">
         <v>1</v>
@@ -2364,11 +2363,11 @@
       </c>
       <c r="S5" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M5,Trigger),"--")</f>
-        <v>42184</v>
+        <v>42283</v>
       </c>
       <c r="T5" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M5,Trigger),"--")</f>
-        <v>42185</v>
+        <v>42284</v>
       </c>
       <c r="U5" s="159"/>
       <c r="V5" s="3" t="str">
@@ -2376,7 +2375,7 @@
         <v>Dp</v>
       </c>
       <c r="W5" s="3" t="str">
-        <v>obj_00264</v>
+        <v>obj_002a8</v>
       </c>
       <c r="X5" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W5,Trigger),"")</f>
@@ -2384,7 +2383,7 @@
       </c>
       <c r="Y5" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W5,Trigger),"")</f>
-        <v>2.2300000000000004E-2</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="Z5" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W5)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W5)),_xll.qlSwapRateHelperSpread($W5))</f>
@@ -2392,14 +2391,14 @@
       </c>
       <c r="AA5" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W5,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB5" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W5,Trigger),"")</f>
-        <v>42187</v>
+        <v>42285</v>
       </c>
       <c r="AC5" s="68">
-        <v>2.229523282489658E-2</v>
+        <v>2.3294795755764795E-2</v>
       </c>
       <c r="AD5" s="158"/>
       <c r="AE5" s="103" t="s">
@@ -2431,7 +2430,7 @@
       </c>
       <c r="G6" s="55" t="str">
         <f>_xll.qlIborIndex(,FamilyName,C6,0,Currency,Calendar,E6,D6,F6,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00255#0000</v>
+        <v>obj_0029a#0002</v>
       </c>
       <c r="H6" s="153" t="str">
         <f t="shared" si="0"/>
@@ -2440,7 +2439,7 @@
       <c r="I6" s="127"/>
       <c r="J6" s="57" t="str">
         <f>_xll.qlDepositRateHelper(,H6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00264#0000</v>
+        <v>obj_002a8#0002</v>
       </c>
       <c r="K6" s="48"/>
       <c r="L6" s="9" t="str">
@@ -2449,7 +2448,7 @@
       </c>
       <c r="M6" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_00264#0000</v>
+        <v>obj_002a8#0002</v>
       </c>
       <c r="N6" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M6,Trigger),"--")</f>
@@ -2457,7 +2456,7 @@
       </c>
       <c r="O6" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M6,Trigger),"--")</f>
-        <v>2.2300000000000004E-2</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="P6" s="93" t="b">
         <v>1</v>
@@ -2470,11 +2469,11 @@
       </c>
       <c r="S6" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M6,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T6" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M6,Trigger),"--")</f>
-        <v>42187</v>
+        <v>42285</v>
       </c>
       <c r="U6" s="159"/>
       <c r="V6" s="3" t="str">
@@ -2482,7 +2481,7 @@
         <v>Dp</v>
       </c>
       <c r="W6" s="3" t="str">
-        <v>obj_0025b</v>
+        <v>obj_002a4</v>
       </c>
       <c r="X6" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W6,Trigger),"")</f>
@@ -2490,7 +2489,7 @@
       </c>
       <c r="Y6" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W6,Trigger),"")</f>
-        <v>2.3E-2</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="Z6" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W6)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W6)),_xll.qlSwapRateHelperSpread($W6))</f>
@@ -2498,14 +2497,14 @@
       </c>
       <c r="AA6" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W6,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB6" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W6,Trigger),"")</f>
-        <v>42194</v>
+        <v>42292</v>
       </c>
       <c r="AC6" s="68">
-        <v>2.2989860757249854E-2</v>
+        <v>2.3289594610018081E-2</v>
       </c>
       <c r="AD6" s="158"/>
       <c r="AE6" s="103" t="s">
@@ -2538,7 +2537,7 @@
       </c>
       <c r="G7" s="60" t="str">
         <f>_xll.qlIborIndex(,FamilyName,C7,0,Currency,Calendar,E7,D7,F7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025a#0000</v>
+        <v>obj_002a3#0002</v>
       </c>
       <c r="H7" s="118" t="str">
         <f t="shared" si="0"/>
@@ -2547,7 +2546,7 @@
       <c r="I7" s="121"/>
       <c r="J7" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H7,G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025b#0000</v>
+        <v>obj_002a4#0002</v>
       </c>
       <c r="K7" s="48"/>
       <c r="L7" s="9" t="str">
@@ -2556,7 +2555,7 @@
       </c>
       <c r="M7" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_0025b#0000</v>
+        <v>obj_002a4#0002</v>
       </c>
       <c r="N7" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M7,Trigger),"--")</f>
@@ -2564,7 +2563,7 @@
       </c>
       <c r="O7" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M7,Trigger),"--")</f>
-        <v>2.3E-2</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="P7" s="93" t="b">
         <v>1</v>
@@ -2577,11 +2576,11 @@
       </c>
       <c r="S7" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M7,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T7" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M7,Trigger),"--")</f>
-        <v>42194</v>
+        <v>42292</v>
       </c>
       <c r="U7" s="159"/>
       <c r="V7" s="3" t="str">
@@ -2589,7 +2588,7 @@
         <v>Dp</v>
       </c>
       <c r="W7" s="3" t="str">
-        <v>obj_0025e</v>
+        <v>obj_002a2</v>
       </c>
       <c r="X7" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W7,Trigger),"")</f>
@@ -2597,7 +2596,7 @@
       </c>
       <c r="Y7" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W7,Trigger),"")</f>
-        <v>2.2700000000000001E-2</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="Z7" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W7)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W7)),_xll.qlSwapRateHelperSpread($W7))</f>
@@ -2605,14 +2604,14 @@
       </c>
       <c r="AA7" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W7,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB7" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W7,Trigger),"")</f>
-        <v>42201</v>
+        <v>42299</v>
       </c>
       <c r="AC7" s="68">
-        <v>2.2685189482931776E-2</v>
+        <v>2.3284396559652587E-2</v>
       </c>
       <c r="AD7" s="158"/>
       <c r="AH7" s="156"/>
@@ -2639,7 +2638,7 @@
       </c>
       <c r="G8" s="6" t="str">
         <f>_xll.qlIborIndex(,FamilyName,C8,0,Currency,Calendar,E8,D8,F8,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00259#0000</v>
+        <v>obj_002a1#0002</v>
       </c>
       <c r="H8" s="119" t="str">
         <f t="shared" si="0"/>
@@ -2648,7 +2647,7 @@
       <c r="I8" s="122"/>
       <c r="J8" s="2" t="str">
         <f>_xll.qlDepositRateHelper(,H8,G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025e#0000</v>
+        <v>obj_002a2#0002</v>
       </c>
       <c r="K8" s="48"/>
       <c r="L8" s="9" t="str">
@@ -2657,7 +2656,7 @@
       </c>
       <c r="M8" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_0025e#0000</v>
+        <v>obj_002a2#0002</v>
       </c>
       <c r="N8" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M8,Trigger),"--")</f>
@@ -2665,7 +2664,7 @@
       </c>
       <c r="O8" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M8,Trigger),"--")</f>
-        <v>2.2700000000000001E-2</v>
+        <v>2.3300000000000001E-2</v>
       </c>
       <c r="P8" s="93" t="b">
         <v>1</v>
@@ -2678,11 +2677,11 @@
       </c>
       <c r="S8" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M8,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T8" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M8,Trigger),"--")</f>
-        <v>42201</v>
+        <v>42299</v>
       </c>
       <c r="U8" s="159"/>
       <c r="V8" s="3" t="str">
@@ -2690,7 +2689,7 @@
         <v>Dp</v>
       </c>
       <c r="W8" s="3" t="str">
-        <v>obj_0025f</v>
+        <v>obj_0029e</v>
       </c>
       <c r="X8" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W8,Trigger),"")</f>
@@ -2698,7 +2697,7 @@
       </c>
       <c r="Y8" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W8,Trigger),"")</f>
-        <v>2.0400000000000001E-2</v>
+        <v>2.0599999999999997E-2</v>
       </c>
       <c r="Z8" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W8)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W8)),_xll.qlSwapRateHelperSpread($W8))</f>
@@ -2706,14 +2705,14 @@
       </c>
       <c r="AA8" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W8,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB8" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W8,Trigger),"")</f>
-        <v>42212</v>
+        <v>42310</v>
       </c>
       <c r="AC8" s="68">
-        <v>2.0381779091941749E-2</v>
+        <v>2.058142028476127E-2</v>
       </c>
       <c r="AD8" s="158"/>
       <c r="AH8" s="156"/>
@@ -2743,7 +2742,7 @@
       <c r="I9" s="121"/>
       <c r="J9" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H9,G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025f#0000</v>
+        <v>obj_0029e#0002</v>
       </c>
       <c r="K9" s="48"/>
       <c r="L9" s="9" t="str">
@@ -2752,7 +2751,7 @@
       </c>
       <c r="M9" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_0025f#0000</v>
+        <v>obj_0029e#0002</v>
       </c>
       <c r="N9" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M9,Trigger),"--")</f>
@@ -2760,7 +2759,7 @@
       </c>
       <c r="O9" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M9,Trigger),"--")</f>
-        <v>2.0400000000000001E-2</v>
+        <v>2.0599999999999997E-2</v>
       </c>
       <c r="P9" s="93" t="b">
         <v>1</v>
@@ -2773,11 +2772,11 @@
       </c>
       <c r="S9" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M9,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T9" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M9,Trigger),"--")</f>
-        <v>42212</v>
+        <v>42310</v>
       </c>
       <c r="U9" s="159"/>
       <c r="V9" s="3" t="str">
@@ -2785,7 +2784,7 @@
         <v>Dp</v>
       </c>
       <c r="W9" s="3" t="str">
-        <v>obj_00256</v>
+        <v>obj_0029d</v>
       </c>
       <c r="X9" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W9,Trigger),"")</f>
@@ -2793,7 +2792,7 @@
       </c>
       <c r="Y9" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W9,Trigger),"")</f>
-        <v>2.1050000000000003E-2</v>
+        <v>2.1299999999999999E-2</v>
       </c>
       <c r="Z9" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W9)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W9)),_xll.qlSwapRateHelperSpread($W9))</f>
@@ -2801,14 +2800,14 @@
       </c>
       <c r="AA9" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W9,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB9" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W9,Trigger),"")</f>
-        <v>42241</v>
+        <v>42339</v>
       </c>
       <c r="AC9" s="68">
-        <v>2.1013060236072151E-2</v>
+        <v>2.1262178647003426E-2</v>
       </c>
       <c r="AD9" s="158"/>
       <c r="AH9" s="156"/>
@@ -2838,7 +2837,7 @@
       <c r="I10" s="121"/>
       <c r="J10" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H10,G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00256#0000</v>
+        <v>obj_0029d#0002</v>
       </c>
       <c r="K10" s="48" t="s">
         <v>34</v>
@@ -2849,7 +2848,7 @@
       </c>
       <c r="M10" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_00256#0000</v>
+        <v>obj_0029d#0002</v>
       </c>
       <c r="N10" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M10,Trigger),"--")</f>
@@ -2857,7 +2856,7 @@
       </c>
       <c r="O10" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M10,Trigger),"--")</f>
-        <v>2.1050000000000003E-2</v>
+        <v>2.1299999999999999E-2</v>
       </c>
       <c r="P10" s="93" t="b">
         <v>1</v>
@@ -2870,11 +2869,11 @@
       </c>
       <c r="S10" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M10,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T10" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M10,Trigger),"--")</f>
-        <v>42241</v>
+        <v>42339</v>
       </c>
       <c r="U10" s="159"/>
       <c r="V10" s="3" t="str">
@@ -2882,7 +2881,7 @@
         <v>Dp</v>
       </c>
       <c r="W10" s="3" t="str">
-        <v>obj_00258</v>
+        <v>obj_002a0</v>
       </c>
       <c r="X10" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W10,Trigger),"")</f>
@@ -2898,14 +2897,14 @@
       </c>
       <c r="AA10" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W10,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB10" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W10,Trigger),"")</f>
-        <v>42272</v>
+        <v>42373</v>
       </c>
       <c r="AC10" s="68">
-        <v>2.1591142150516409E-2</v>
+        <v>2.1589230049233528E-2</v>
       </c>
       <c r="AD10" s="158"/>
       <c r="AH10" s="156"/>
@@ -2935,7 +2934,7 @@
       <c r="I11" s="121"/>
       <c r="J11" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H11,G11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00258#0000</v>
+        <v>obj_002a0#0002</v>
       </c>
       <c r="K11" s="48"/>
       <c r="L11" s="9" t="str">
@@ -2944,7 +2943,7 @@
       </c>
       <c r="M11" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_00258#0000</v>
+        <v>obj_002a0#0002</v>
       </c>
       <c r="N11" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M11,Trigger),"--")</f>
@@ -2965,11 +2964,11 @@
       </c>
       <c r="S11" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M11,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T11" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M11,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42373</v>
       </c>
       <c r="U11" s="159"/>
       <c r="V11" s="3" t="str">
@@ -2977,7 +2976,7 @@
         <v>Dp</v>
       </c>
       <c r="W11" s="3" t="str">
-        <v>obj_0025c</v>
+        <v>obj_0029b</v>
       </c>
       <c r="X11" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W11,Trigger),"")</f>
@@ -2985,7 +2984,7 @@
       </c>
       <c r="Y11" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W11,Trigger),"")</f>
-        <v>2.1900000000000003E-2</v>
+        <v>2.1950000000000004E-2</v>
       </c>
       <c r="Z11" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W11)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W11)),_xll.qlSwapRateHelperSpread($W11))</f>
@@ -2993,14 +2992,14 @@
       </c>
       <c r="AA11" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W11,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB11" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W11,Trigger),"")</f>
-        <v>42303</v>
+        <v>42401</v>
       </c>
       <c r="AC11" s="68">
-        <v>2.1819584402372163E-2</v>
+        <v>2.1869217690562687E-2</v>
       </c>
       <c r="AD11" s="158"/>
       <c r="AH11" s="156"/>
@@ -3030,7 +3029,7 @@
       <c r="I12" s="121"/>
       <c r="J12" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H12,G12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025c#0000</v>
+        <v>obj_0029b#0002</v>
       </c>
       <c r="K12" s="48"/>
       <c r="L12" s="9" t="str">
@@ -3039,7 +3038,7 @@
       </c>
       <c r="M12" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_0025c#0000</v>
+        <v>obj_0029b#0002</v>
       </c>
       <c r="N12" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M12,Trigger),"--")</f>
@@ -3047,7 +3046,7 @@
       </c>
       <c r="O12" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M12,Trigger),"--")</f>
-        <v>2.1900000000000003E-2</v>
+        <v>2.1950000000000004E-2</v>
       </c>
       <c r="P12" s="93" t="b">
         <v>1</v>
@@ -3060,18 +3059,18 @@
       </c>
       <c r="S12" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M12,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T12" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M12,Trigger),"--")</f>
-        <v>42303</v>
+        <v>42401</v>
       </c>
       <c r="V12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Dp</v>
       </c>
       <c r="W12" s="3" t="str">
-        <v>obj_0025d</v>
+        <v>obj_0029c</v>
       </c>
       <c r="X12" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W12,Trigger),"")</f>
@@ -3079,7 +3078,7 @@
       </c>
       <c r="Y12" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W12,Trigger),"")</f>
-        <v>2.2199999999999998E-2</v>
+        <v>2.205E-2</v>
       </c>
       <c r="Z12" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W12)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W12)),_xll.qlSwapRateHelperSpread($W12))</f>
@@ -3087,14 +3086,14 @@
       </c>
       <c r="AA12" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W12,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB12" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W12,Trigger),"")</f>
-        <v>42333</v>
+        <v>42430</v>
       </c>
       <c r="AC12" s="68">
-        <v>2.2097342515700464E-2</v>
+        <v>2.1949378813090337E-2</v>
       </c>
       <c r="AD12" s="158"/>
       <c r="AH12" s="156"/>
@@ -3124,7 +3123,7 @@
       <c r="I13" s="121"/>
       <c r="J13" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H13,G13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0025d#0000</v>
+        <v>obj_0029c#0002</v>
       </c>
       <c r="K13" s="48"/>
       <c r="L13" s="9" t="str">
@@ -3133,7 +3132,7 @@
       </c>
       <c r="M13" s="90" t="str">
         <f t="shared" si="2"/>
-        <v>obj_0025d#0000</v>
+        <v>obj_0029c#0002</v>
       </c>
       <c r="N13" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M13,Trigger),"--")</f>
@@ -3141,7 +3140,7 @@
       </c>
       <c r="O13" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M13,Trigger),"--")</f>
-        <v>2.2199999999999998E-2</v>
+        <v>2.205E-2</v>
       </c>
       <c r="P13" s="93" t="b">
         <v>1</v>
@@ -3154,18 +3153,18 @@
       </c>
       <c r="S13" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M13,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T13" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M13,Trigger),"--")</f>
-        <v>42333</v>
+        <v>42430</v>
       </c>
       <c r="V13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Dp</v>
       </c>
       <c r="W13" s="3" t="str">
-        <v>obj_00257</v>
+        <v>obj_0029f</v>
       </c>
       <c r="X13" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W13,Trigger),"")</f>
@@ -3173,7 +3172,7 @@
       </c>
       <c r="Y13" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W13,Trigger),"")</f>
-        <v>2.2717000000000001E-2</v>
+        <v>2.2400000000000003E-2</v>
       </c>
       <c r="Z13" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W13)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W13)),_xll.qlSwapRateHelperSpread($W13))</f>
@@ -3181,14 +3180,14 @@
       </c>
       <c r="AA13" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W13,Trigger),"")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="AB13" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W13,Trigger),"")</f>
-        <v>42367</v>
+        <v>42461</v>
       </c>
       <c r="AC13" s="68">
-        <v>2.2585820123008367E-2</v>
+        <v>2.2275150224777981E-2</v>
       </c>
       <c r="AD13" s="158"/>
       <c r="AH13" s="156"/>
@@ -3218,7 +3217,7 @@
       <c r="I14" s="122"/>
       <c r="J14" s="2" t="str">
         <f>_xll.qlDepositRateHelper(,H14,G14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00257#0000</v>
+        <v>obj_0029f#0002</v>
       </c>
       <c r="K14" s="48"/>
       <c r="L14" s="10" t="str">
@@ -3227,7 +3226,7 @@
       </c>
       <c r="M14" s="91" t="str">
         <f t="shared" si="2"/>
-        <v>obj_00257#0000</v>
+        <v>obj_0029f#0002</v>
       </c>
       <c r="N14" s="144" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M14,Trigger),"--")</f>
@@ -3235,7 +3234,7 @@
       </c>
       <c r="O14" s="97">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M14,Trigger),"--")</f>
-        <v>2.2717000000000001E-2</v>
+        <v>2.2400000000000003E-2</v>
       </c>
       <c r="P14" s="96" t="b">
         <v>1</v>
@@ -3248,26 +3247,26 @@
       </c>
       <c r="S14" s="98">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M14,Trigger),"--")</f>
-        <v>42180</v>
+        <v>42278</v>
       </c>
       <c r="T14" s="98">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M14,Trigger),"--")</f>
-        <v>42367</v>
+        <v>42461</v>
       </c>
       <c r="V14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>FUT</v>
       </c>
       <c r="W14" s="3" t="str">
-        <v>obj_0026b</v>
+        <v>obj_002ab</v>
       </c>
       <c r="X14" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W14,Trigger),"")</f>
-        <v>AUDFUT3MH6_Quote</v>
+        <v>AUDFUT3MM6_Quote</v>
       </c>
       <c r="Y14" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W14,Trigger),"")</f>
-        <v>2.1049999999999902E-2</v>
+        <v>1.8549999999999844E-2</v>
       </c>
       <c r="Z14" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W14)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W14)),_xll.qlSwapRateHelperSpread($W14))</f>
@@ -3275,14 +3274,14 @@
       </c>
       <c r="AA14" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W14,Trigger),"")</f>
-        <v>42440</v>
+        <v>42531</v>
       </c>
       <c r="AB14" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W14,Trigger),"")</f>
-        <v>42535</v>
+        <v>42625</v>
       </c>
       <c r="AC14" s="68">
-        <v>2.1960422698838626E-2</v>
+        <v>2.0792732318726463E-2</v>
       </c>
       <c r="AD14" s="158"/>
       <c r="AH14" s="156"/>
@@ -3306,11 +3305,11 @@
       </c>
       <c r="M15" s="128" t="str">
         <f t="shared" ref="M15:M36" si="7">IF(ISBLANK(J17),"--",J17)</f>
-        <v>obj_00265#0000</v>
+        <v>obj_002bb#0002</v>
       </c>
       <c r="N15" s="142" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M15,Trigger),"--")</f>
-        <v>AUDFUT3MN5_Quote</v>
+        <v>AUDFUT3MV5_Quote</v>
       </c>
       <c r="O15" s="147" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M15,Trigger),"--")</f>
@@ -3327,26 +3326,26 @@
       </c>
       <c r="S15" s="131">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M15,Trigger),"--")</f>
-        <v>42195</v>
+        <v>42286</v>
       </c>
       <c r="T15" s="131">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M15,Trigger),"--")</f>
-        <v>42289</v>
+        <v>42380</v>
       </c>
       <c r="V15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>FUT</v>
       </c>
       <c r="W15" s="3" t="str">
-        <v>obj_0026c</v>
+        <v>obj_002b1</v>
       </c>
       <c r="X15" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W15,Trigger),"")</f>
-        <v>AUDFUT3MM6_Quote</v>
+        <v>AUDFUT3MU6_Quote</v>
       </c>
       <c r="Y15" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W15,Trigger),"")</f>
-        <v>2.1299999999999986E-2</v>
+        <v>1.8549999999999844E-2</v>
       </c>
       <c r="Z15" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W15)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W15)),_xll.qlSwapRateHelperSpread($W15))</f>
@@ -3354,14 +3353,14 @@
       </c>
       <c r="AA15" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W15,Trigger),"")</f>
-        <v>42531</v>
+        <v>42622</v>
       </c>
       <c r="AB15" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W15,Trigger),"")</f>
-        <v>42625</v>
+        <v>42713</v>
       </c>
       <c r="AC15" s="68">
-        <v>2.1820367167677556E-2</v>
+        <v>2.0336061735131722E-2</v>
       </c>
       <c r="AD15" s="158"/>
       <c r="AH15" s="156"/>
@@ -3398,11 +3397,11 @@
       </c>
       <c r="M16" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00266#0000</v>
+        <v>obj_002b0#0002</v>
       </c>
       <c r="N16" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M16,Trigger),"--")</f>
-        <v>AUDFUT3MQ5_Quote</v>
+        <v>AUDFUT3MX5_Quote</v>
       </c>
       <c r="O16" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M16,Trigger),"--")</f>
@@ -3419,26 +3418,26 @@
       </c>
       <c r="S16" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M16,Trigger),"--")</f>
-        <v>42230</v>
+        <v>42321</v>
       </c>
       <c r="T16" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M16,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42415</v>
       </c>
       <c r="V16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>FUT</v>
       </c>
       <c r="W16" s="3" t="str">
-        <v>obj_0026d</v>
+        <v>obj_002ba</v>
       </c>
       <c r="X16" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W16,Trigger),"")</f>
-        <v>AUDFUT3MU6_Quote</v>
+        <v>AUDFUT3MZ6_Quote</v>
       </c>
       <c r="Y16" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W16,Trigger),"")</f>
-        <v>2.1900000000000031E-2</v>
+        <v>1.8849999999999922E-2</v>
       </c>
       <c r="Z16" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W16)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W16)),_xll.qlSwapRateHelperSpread($W16))</f>
@@ -3446,14 +3445,14 @@
       </c>
       <c r="AA16" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W16,Trigger),"")</f>
-        <v>42622</v>
+        <v>42713</v>
       </c>
       <c r="AB16" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W16,Trigger),"")</f>
-        <v>42713</v>
+        <v>42803</v>
       </c>
       <c r="AC16" s="68">
-        <v>2.1827663938347251E-2</v>
+        <v>2.0073821732480363E-2</v>
       </c>
       <c r="AD16" s="158"/>
       <c r="AH16" s="156"/>
@@ -3467,7 +3466,7 @@
       </c>
       <c r="C17" s="56" t="str">
         <f>_xll.qlASXNextCode(Evaluationdate-1,B17,Trigger)</f>
-        <v>N5</v>
+        <v>V5</v>
       </c>
       <c r="D17" s="127"/>
       <c r="E17" s="127"/>
@@ -3478,15 +3477,15 @@
       </c>
       <c r="H17" s="114" t="str">
         <f t="shared" ref="H17:H38" si="9">Currency&amp;"FUT"&amp;$G$15&amp;$C17&amp;QuoteSuffix</f>
-        <v>AUDFUT3MN5_Quote</v>
+        <v>AUDFUT3MV5_Quote</v>
       </c>
       <c r="I17" s="114" t="str">
         <f t="shared" ref="I17:I38" si="10">Currency&amp;"FUT"&amp;$G$15&amp;$C17&amp;"ConvAdj"&amp;QuoteSuffix</f>
-        <v>AUDFUT3MN5ConvAdj_Quote</v>
+        <v>AUDFUT3MV5ConvAdj_Quote</v>
       </c>
       <c r="J17" s="57" t="str">
         <f>_xll.qlFuturesRateHelper(,H17,$H$15,_xll.qlASXdate(C17),G17,I17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00265#0000</v>
+        <v>obj_002bb#0002</v>
       </c>
       <c r="K17" s="48"/>
       <c r="L17" s="9" t="str">
@@ -3495,15 +3494,15 @@
       </c>
       <c r="M17" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00267#0000</v>
+        <v>obj_002b2#0002</v>
       </c>
       <c r="N17" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M17,Trigger),"--")</f>
-        <v>AUDFUT3MU5_Quote</v>
+        <v>AUDFUT3MZ5_Quote</v>
       </c>
       <c r="O17" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M17,Trigger),"--")</f>
-        <v>97.875</v>
+        <v>97.954999999999998</v>
       </c>
       <c r="P17" s="93" t="b">
         <v>0</v>
@@ -3516,26 +3515,26 @@
       </c>
       <c r="S17" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M17,Trigger),"--")</f>
-        <v>42258</v>
+        <v>42349</v>
       </c>
       <c r="T17" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M17,Trigger),"--")</f>
-        <v>42349</v>
+        <v>42440</v>
       </c>
       <c r="V17" s="3" t="str">
         <f t="shared" si="3"/>
         <v>FUT</v>
       </c>
       <c r="W17" s="3" t="str">
-        <v>obj_0026e</v>
+        <v>obj_002ae</v>
       </c>
       <c r="X17" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W17,Trigger),"")</f>
-        <v>AUDFUT3MZ6_Quote</v>
+        <v>AUDFUT3MH7_Quote</v>
       </c>
       <c r="Y17" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W17,Trigger),"")</f>
-        <v>2.2699999999999942E-2</v>
+        <v>1.9449999999999967E-2</v>
       </c>
       <c r="Z17" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W17)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W17)),_xll.qlSwapRateHelperSpread($W17))</f>
@@ -3543,14 +3542,14 @@
       </c>
       <c r="AA17" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W17,Trigger),"")</f>
-        <v>42713</v>
+        <v>42804</v>
       </c>
       <c r="AB17" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W17,Trigger),"")</f>
-        <v>42803</v>
+        <v>42899</v>
       </c>
       <c r="AC17" s="68">
-        <v>2.1944540166973819E-2</v>
+        <v>1.9969967735023582E-2</v>
       </c>
       <c r="AD17" s="158"/>
       <c r="AH17" s="156"/>
@@ -3564,7 +3563,7 @@
       </c>
       <c r="C18" s="61" t="str">
         <f>_xll.qlASXNextCode(C17,B18,Trigger)</f>
-        <v>Q5</v>
+        <v>X5</v>
       </c>
       <c r="D18" s="121"/>
       <c r="E18" s="121"/>
@@ -3575,15 +3574,15 @@
       </c>
       <c r="H18" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MQ5_Quote</v>
+        <v>AUDFUT3MX5_Quote</v>
       </c>
       <c r="I18" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MQ5ConvAdj_Quote</v>
+        <v>AUDFUT3MX5ConvAdj_Quote</v>
       </c>
       <c r="J18" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H18,$H$15,_xll.qlASXdate(C18),G18,I18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00266#0000</v>
+        <v>obj_002b0#0002</v>
       </c>
       <c r="K18" s="48"/>
       <c r="L18" s="9" t="str">
@@ -3592,11 +3591,11 @@
       </c>
       <c r="M18" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00268#0000</v>
+        <v>obj_002b6#0002</v>
       </c>
       <c r="N18" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M18,Trigger),"--")</f>
-        <v>AUDFUT3MV5_Quote</v>
+        <v>AUDFUT3MF6_Quote</v>
       </c>
       <c r="O18" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M18,Trigger),"--")</f>
@@ -3613,18 +3612,18 @@
       </c>
       <c r="S18" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M18,Trigger),"--")</f>
-        <v>42286</v>
+        <v>42377</v>
       </c>
       <c r="T18" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M18,Trigger),"--")</f>
-        <v>42380</v>
+        <v>42468</v>
       </c>
       <c r="V18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W18" s="3" t="str">
-        <v>obj_00261</v>
+        <v>obj_002a7</v>
       </c>
       <c r="X18" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W18,Trigger),"")</f>
@@ -3632,7 +3631,7 @@
       </c>
       <c r="Y18" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W18,Trigger),"")</f>
-        <v>2.1925E-2</v>
+        <v>1.9675000000000002E-2</v>
       </c>
       <c r="Z18" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W18)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W18)),_xll.qlSwapRateHelperSpread($W18))</f>
@@ -3640,14 +3639,14 @@
       </c>
       <c r="AA18" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W18,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB18" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W18,Trigger),"")</f>
-        <v>42912</v>
+        <v>43011</v>
       </c>
       <c r="AC18" s="68">
-        <v>2.1863946311077673E-2</v>
+        <v>1.9615941759067567E-2</v>
       </c>
       <c r="AD18" s="158"/>
       <c r="AH18" s="156"/>
@@ -3661,7 +3660,7 @@
       </c>
       <c r="C19" s="61" t="str">
         <f>_xll.qlASXNextCode(C18,B19,Trigger)</f>
-        <v>U5</v>
+        <v>Z5</v>
       </c>
       <c r="D19" s="121"/>
       <c r="E19" s="121"/>
@@ -3672,15 +3671,15 @@
       </c>
       <c r="H19" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MU5_Quote</v>
+        <v>AUDFUT3MZ5_Quote</v>
       </c>
       <c r="I19" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MU5ConvAdj_Quote</v>
+        <v>AUDFUT3MZ5ConvAdj_Quote</v>
       </c>
       <c r="J19" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H19,$H$15,_xll.qlASXdate(C19),G19,I19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00267#0000</v>
+        <v>obj_002b2#0002</v>
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="9" t="str">
@@ -3689,11 +3688,11 @@
       </c>
       <c r="M19" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00269#0000</v>
+        <v>obj_002b5#0002</v>
       </c>
       <c r="N19" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M19,Trigger),"--")</f>
-        <v>AUDFUT3MX5_Quote</v>
+        <v>AUDFUT3MG6_Quote</v>
       </c>
       <c r="O19" s="148" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M19,Trigger),"--")</f>
@@ -3710,18 +3709,18 @@
       </c>
       <c r="S19" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M19,Trigger),"--")</f>
-        <v>42321</v>
+        <v>42412</v>
       </c>
       <c r="T19" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M19,Trigger),"--")</f>
-        <v>42415</v>
+        <v>42502</v>
       </c>
       <c r="V19" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W19" s="3" t="str">
-        <v>obj_00262</v>
+        <v>obj_002a6</v>
       </c>
       <c r="X19" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W19,Trigger),"")</f>
@@ -3729,7 +3728,7 @@
       </c>
       <c r="Y19" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W19,Trigger),"")</f>
-        <v>2.3349999999999999E-2</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="Z19" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W19)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W19)),_xll.qlSwapRateHelperSpread($W19))</f>
@@ -3737,14 +3736,14 @@
       </c>
       <c r="AA19" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W19,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB19" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W19,Trigger),"")</f>
-        <v>43277</v>
+        <v>43375</v>
       </c>
       <c r="AC19" s="68">
-        <v>2.3315381291721657E-2</v>
+        <v>2.0355658485432779E-2</v>
       </c>
       <c r="AD19" s="158"/>
       <c r="AH19" s="156"/>
@@ -3758,7 +3757,7 @@
       </c>
       <c r="C20" s="61" t="str">
         <f>_xll.qlASXNextCode(C19,B20,Trigger)</f>
-        <v>V5</v>
+        <v>F6</v>
       </c>
       <c r="D20" s="121"/>
       <c r="E20" s="121"/>
@@ -3769,15 +3768,15 @@
       </c>
       <c r="H20" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MV5_Quote</v>
+        <v>AUDFUT3MF6_Quote</v>
       </c>
       <c r="I20" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MV5ConvAdj_Quote</v>
+        <v>AUDFUT3MF6ConvAdj_Quote</v>
       </c>
       <c r="J20" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H20,$H$15,_xll.qlASXdate(C20),G20,I20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00268#0000</v>
+        <v>obj_002b6#0002</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="9" t="str">
@@ -3786,15 +3785,15 @@
       </c>
       <c r="M20" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0026a#0000</v>
+        <v>obj_002af#0002</v>
       </c>
       <c r="N20" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M20,Trigger),"--")</f>
-        <v>AUDFUT3MZ5_Quote</v>
+        <v>AUDFUT3MH6_Quote</v>
       </c>
       <c r="O20" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M20,Trigger),"--")</f>
-        <v>97.89500000000001</v>
+        <v>98.085000000000008</v>
       </c>
       <c r="P20" s="93" t="b">
         <v>0</v>
@@ -3807,18 +3806,18 @@
       </c>
       <c r="S20" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M20,Trigger),"--")</f>
-        <v>42349</v>
+        <v>42440</v>
       </c>
       <c r="T20" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M20,Trigger),"--")</f>
-        <v>42440</v>
+        <v>42535</v>
       </c>
       <c r="V20" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W20" s="3" t="str">
-        <v>obj_00253</v>
+        <v>obj_00296</v>
       </c>
       <c r="X20" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W20,Trigger),"")</f>
@@ -3826,7 +3825,7 @@
       </c>
       <c r="Y20" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W20,Trigger),"")</f>
-        <v>2.6050000000000004E-2</v>
+        <v>2.2675000000000001E-2</v>
       </c>
       <c r="Z20" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W20)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W20)),_xll.qlSwapRateHelperSpread($W20))</f>
@@ -3834,14 +3833,14 @@
       </c>
       <c r="AA20" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W20,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB20" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W20,Trigger),"")</f>
-        <v>43642</v>
+        <v>43740</v>
       </c>
       <c r="AC20" s="68">
-        <v>2.6014050769013464E-2</v>
+        <v>2.2630177977450823E-2</v>
       </c>
       <c r="AD20" s="158"/>
       <c r="AH20" s="156"/>
@@ -3855,7 +3854,7 @@
       </c>
       <c r="C21" s="8" t="str">
         <f>_xll.qlASXNextCode(C20,B21,Trigger)</f>
-        <v>X5</v>
+        <v>G6</v>
       </c>
       <c r="D21" s="122"/>
       <c r="E21" s="122"/>
@@ -3866,15 +3865,15 @@
       </c>
       <c r="H21" s="116" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MX5_Quote</v>
+        <v>AUDFUT3MG6_Quote</v>
       </c>
       <c r="I21" s="116" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MX5ConvAdj_Quote</v>
+        <v>AUDFUT3MG6ConvAdj_Quote</v>
       </c>
       <c r="J21" s="2" t="str">
         <f>_xll.qlFuturesRateHelper(,H21,$H$15,_xll.qlASXdate(C21),G21,I21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00269#0000</v>
+        <v>obj_002b5#0002</v>
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="9" t="str">
@@ -3883,15 +3882,15 @@
       </c>
       <c r="M21" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0026b#0000</v>
+        <v>obj_002ab#0002</v>
       </c>
       <c r="N21" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M21,Trigger),"--")</f>
-        <v>AUDFUT3MH6_Quote</v>
+        <v>AUDFUT3MM6_Quote</v>
       </c>
       <c r="O21" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M21,Trigger),"--")</f>
-        <v>97.89500000000001</v>
+        <v>98.14500000000001</v>
       </c>
       <c r="P21" s="93" t="b">
         <v>1</v>
@@ -3904,18 +3903,18 @@
       </c>
       <c r="S21" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M21,Trigger),"--")</f>
-        <v>42440</v>
+        <v>42531</v>
       </c>
       <c r="T21" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M21,Trigger),"--")</f>
-        <v>42535</v>
+        <v>42625</v>
       </c>
       <c r="V21" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W21" s="3" t="str">
-        <v>obj_0024b</v>
+        <v>obj_00291</v>
       </c>
       <c r="X21" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W21,Trigger),"")</f>
@@ -3923,7 +3922,7 @@
       </c>
       <c r="Y21" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W21,Trigger),"")</f>
-        <v>2.7824999999999999E-2</v>
+        <v>2.3975E-2</v>
       </c>
       <c r="Z21" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W21)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W21)),_xll.qlSwapRateHelperSpread($W21))</f>
@@ -3931,14 +3930,14 @@
       </c>
       <c r="AA21" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W21,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB21" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W21,Trigger),"")</f>
-        <v>44008</v>
+        <v>44106</v>
       </c>
       <c r="AC21" s="68">
-        <v>2.7848642276123055E-2</v>
+        <v>2.3966441921497626E-2</v>
       </c>
       <c r="AD21" s="158"/>
       <c r="AH21" s="156"/>
@@ -3952,7 +3951,7 @@
       </c>
       <c r="C22" s="61" t="str">
         <f>_xll.qlASXNextCode(C21,B22,Trigger)</f>
-        <v>Z5</v>
+        <v>H6</v>
       </c>
       <c r="D22" s="121"/>
       <c r="E22" s="121"/>
@@ -3963,15 +3962,15 @@
       </c>
       <c r="H22" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MZ5_Quote</v>
+        <v>AUDFUT3MH6_Quote</v>
       </c>
       <c r="I22" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MZ5ConvAdj_Quote</v>
+        <v>AUDFUT3MH6ConvAdj_Quote</v>
       </c>
       <c r="J22" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H22,$H$15,_xll.qlASXdate(C22),G22,I22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026a#0000</v>
+        <v>obj_002af#0002</v>
       </c>
       <c r="K22" s="48"/>
       <c r="L22" s="9" t="str">
@@ -3980,15 +3979,15 @@
       </c>
       <c r="M22" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0026c#0000</v>
+        <v>obj_002b1#0002</v>
       </c>
       <c r="N22" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M22,Trigger),"--")</f>
-        <v>AUDFUT3MM6_Quote</v>
+        <v>AUDFUT3MU6_Quote</v>
       </c>
       <c r="O22" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M22,Trigger),"--")</f>
-        <v>97.87</v>
+        <v>98.14500000000001</v>
       </c>
       <c r="P22" s="93" t="b">
         <v>1</v>
@@ -4001,18 +4000,18 @@
       </c>
       <c r="S22" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M22,Trigger),"--")</f>
-        <v>42531</v>
+        <v>42622</v>
       </c>
       <c r="T22" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M22,Trigger),"--")</f>
-        <v>42625</v>
+        <v>42713</v>
       </c>
       <c r="V22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W22" s="3" t="str">
-        <v>obj_0024c</v>
+        <v>obj_00292</v>
       </c>
       <c r="X22" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W22,Trigger),"")</f>
@@ -4020,7 +4019,7 @@
       </c>
       <c r="Y22" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W22,Trigger),"")</f>
-        <v>3.0949999999999998E-2</v>
+        <v>2.6437499999999999E-2</v>
       </c>
       <c r="Z22" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W22)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W22)),_xll.qlSwapRateHelperSpread($W22))</f>
@@ -4028,14 +4027,14 @@
       </c>
       <c r="AA22" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W22,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB22" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W22,Trigger),"")</f>
-        <v>44739</v>
+        <v>44838</v>
       </c>
       <c r="AC22" s="68">
-        <v>3.1148972277847083E-2</v>
+        <v>2.6545759914276261E-2</v>
       </c>
       <c r="AD22" s="158"/>
       <c r="AH22" s="156"/>
@@ -4049,7 +4048,7 @@
       </c>
       <c r="C23" s="61" t="str">
         <f>_xll.qlASXNextCode(C22,B23,Trigger)</f>
-        <v>H6</v>
+        <v>M6</v>
       </c>
       <c r="D23" s="121"/>
       <c r="E23" s="121"/>
@@ -4060,15 +4059,15 @@
       </c>
       <c r="H23" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MH6_Quote</v>
+        <v>AUDFUT3MM6_Quote</v>
       </c>
       <c r="I23" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MH6ConvAdj_Quote</v>
+        <v>AUDFUT3MM6ConvAdj_Quote</v>
       </c>
       <c r="J23" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H23,$H$15,_xll.qlASXdate(C23),G23,I23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026b#0000</v>
+        <v>obj_002ab#0002</v>
       </c>
       <c r="K23" s="48"/>
       <c r="L23" s="9" t="str">
@@ -4077,15 +4076,15 @@
       </c>
       <c r="M23" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0026d#0000</v>
+        <v>obj_002ba#0002</v>
       </c>
       <c r="N23" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M23,Trigger),"--")</f>
-        <v>AUDFUT3MU6_Quote</v>
+        <v>AUDFUT3MZ6_Quote</v>
       </c>
       <c r="O23" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M23,Trigger),"--")</f>
-        <v>97.81</v>
+        <v>98.115000000000009</v>
       </c>
       <c r="P23" s="93" t="b">
         <v>1</v>
@@ -4098,18 +4097,18 @@
       </c>
       <c r="S23" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M23,Trigger),"--")</f>
-        <v>42622</v>
+        <v>42713</v>
       </c>
       <c r="T23" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M23,Trigger),"--")</f>
-        <v>42713</v>
+        <v>42803</v>
       </c>
       <c r="V23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W23" s="3" t="str">
-        <v>obj_00252</v>
+        <v>obj_00295</v>
       </c>
       <c r="X23" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W23,Trigger),"")</f>
@@ -4117,7 +4116,7 @@
       </c>
       <c r="Y23" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W23,Trigger),"")</f>
-        <v>3.4025E-2</v>
+        <v>2.9050000000000003E-2</v>
       </c>
       <c r="Z23" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W23)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W23)),_xll.qlSwapRateHelperSpread($W23))</f>
@@ -4125,14 +4124,14 @@
       </c>
       <c r="AA23" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W23,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB23" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W23,Trigger),"")</f>
-        <v>45834</v>
+        <v>45932</v>
       </c>
       <c r="AC23" s="68">
-        <v>3.449838104808936E-2</v>
+        <v>2.9359574263542996E-2</v>
       </c>
       <c r="AD23" s="158"/>
       <c r="AH23" s="156"/>
@@ -4146,7 +4145,7 @@
       </c>
       <c r="C24" s="61" t="str">
         <f>_xll.qlASXNextCode(C23,B24,Trigger)</f>
-        <v>M6</v>
+        <v>U6</v>
       </c>
       <c r="D24" s="121"/>
       <c r="E24" s="121"/>
@@ -4157,15 +4156,15 @@
       </c>
       <c r="H24" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MM6_Quote</v>
+        <v>AUDFUT3MU6_Quote</v>
       </c>
       <c r="I24" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MM6ConvAdj_Quote</v>
+        <v>AUDFUT3MU6ConvAdj_Quote</v>
       </c>
       <c r="J24" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H24,$H$15,_xll.qlASXdate(C24),G24,I24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026c#0000</v>
+        <v>obj_002b1#0002</v>
       </c>
       <c r="K24" s="48"/>
       <c r="L24" s="9" t="str">
@@ -4174,15 +4173,15 @@
       </c>
       <c r="M24" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0026e#0000</v>
+        <v>obj_002ae#0002</v>
       </c>
       <c r="N24" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M24,Trigger),"--")</f>
-        <v>AUDFUT3MZ6_Quote</v>
+        <v>AUDFUT3MH7_Quote</v>
       </c>
       <c r="O24" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M24,Trigger),"--")</f>
-        <v>97.73</v>
+        <v>98.055000000000007</v>
       </c>
       <c r="P24" s="93" t="b">
         <v>1</v>
@@ -4195,18 +4194,18 @@
       </c>
       <c r="S24" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M24,Trigger),"--")</f>
-        <v>42713</v>
+        <v>42804</v>
       </c>
       <c r="T24" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M24,Trigger),"--")</f>
-        <v>42803</v>
+        <v>42899</v>
       </c>
       <c r="V24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W24" s="3" t="str">
-        <v>obj_00251</v>
+        <v>obj_00294</v>
       </c>
       <c r="X24" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W24,Trigger),"")</f>
@@ -4214,7 +4213,7 @@
       </c>
       <c r="Y24" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W24,Trigger),"")</f>
-        <v>3.5425000000000005E-2</v>
+        <v>3.0250000000000003E-2</v>
       </c>
       <c r="Z24" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W24)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W24)),_xll.qlSwapRateHelperSpread($W24))</f>
@@ -4222,14 +4221,14 @@
       </c>
       <c r="AA24" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W24,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB24" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W24,Trigger),"")</f>
-        <v>46566</v>
+        <v>46665</v>
       </c>
       <c r="AC24" s="68">
-        <v>3.6066336048095032E-2</v>
+        <v>3.0681775648587827E-2</v>
       </c>
       <c r="AD24" s="158"/>
       <c r="AH24" s="156"/>
@@ -4243,7 +4242,7 @@
       </c>
       <c r="C25" s="61" t="str">
         <f>_xll.qlASXNextCode(C24,B25,Trigger)</f>
-        <v>U6</v>
+        <v>Z6</v>
       </c>
       <c r="D25" s="121"/>
       <c r="E25" s="121"/>
@@ -4254,15 +4253,15 @@
       </c>
       <c r="H25" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MU6_Quote</v>
+        <v>AUDFUT3MZ6_Quote</v>
       </c>
       <c r="I25" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MU6ConvAdj_Quote</v>
+        <v>AUDFUT3MZ6ConvAdj_Quote</v>
       </c>
       <c r="J25" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H25,$H$15,_xll.qlASXdate(C25),G25,I25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026d#0000</v>
+        <v>obj_002ba#0002</v>
       </c>
       <c r="K25" s="48"/>
       <c r="L25" s="9" t="str">
@@ -4271,15 +4270,15 @@
       </c>
       <c r="M25" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0026f#0000</v>
+        <v>obj_002bd#0002</v>
       </c>
       <c r="N25" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M25,Trigger),"--")</f>
-        <v>AUDFUT3MH7_Quote</v>
+        <v>AUDFUT3MM7_Quote</v>
       </c>
       <c r="O25" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M25,Trigger),"--")</f>
-        <v>97.63</v>
+        <v>97.984999999999999</v>
       </c>
       <c r="P25" s="93" t="b">
         <v>0</v>
@@ -4292,18 +4291,18 @@
       </c>
       <c r="S25" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M25,Trigger),"--")</f>
-        <v>42804</v>
+        <v>42895</v>
       </c>
       <c r="T25" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M25,Trigger),"--")</f>
-        <v>42899</v>
+        <v>42989</v>
       </c>
       <c r="V25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W25" s="3" t="str">
-        <v>obj_00254</v>
+        <v>obj_00297</v>
       </c>
       <c r="X25" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W25,Trigger),"")</f>
@@ -4311,7 +4310,7 @@
       </c>
       <c r="Y25" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W25,Trigger),"")</f>
-        <v>3.6750000000000005E-2</v>
+        <v>3.1524999999999997E-2</v>
       </c>
       <c r="Z25" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W25)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W25)),_xll.qlSwapRateHelperSpread($W25))</f>
@@ -4319,14 +4318,14 @@
       </c>
       <c r="AA25" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W25,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB25" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W25,Trigger),"")</f>
-        <v>47660</v>
+        <v>47758</v>
       </c>
       <c r="AC25" s="68">
-        <v>3.7569982659807419E-2</v>
+        <v>3.2119129524522887E-2</v>
       </c>
       <c r="AD25" s="158"/>
       <c r="AH25" s="156"/>
@@ -4340,7 +4339,7 @@
       </c>
       <c r="C26" s="61" t="str">
         <f>_xll.qlASXNextCode(C25,B26,Trigger)</f>
-        <v>Z6</v>
+        <v>H7</v>
       </c>
       <c r="D26" s="121"/>
       <c r="E26" s="121"/>
@@ -4351,15 +4350,15 @@
       </c>
       <c r="H26" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MZ6_Quote</v>
+        <v>AUDFUT3MH7_Quote</v>
       </c>
       <c r="I26" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MZ6ConvAdj_Quote</v>
+        <v>AUDFUT3MH7ConvAdj_Quote</v>
       </c>
       <c r="J26" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H26,$H$15,_xll.qlASXdate(C26),G26,I26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026e#0000</v>
+        <v>obj_002ae#0002</v>
       </c>
       <c r="K26" s="48"/>
       <c r="L26" s="9" t="str">
@@ -4368,15 +4367,15 @@
       </c>
       <c r="M26" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00270#0000</v>
+        <v>obj_002bf#0002</v>
       </c>
       <c r="N26" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M26,Trigger),"--")</f>
-        <v>AUDFUT3MM7_Quote</v>
+        <v>AUDFUT3MU7_Quote</v>
       </c>
       <c r="O26" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M26,Trigger),"--")</f>
-        <v>97.52000000000001</v>
+        <v>97.914999999999992</v>
       </c>
       <c r="P26" s="93" t="b">
         <v>0</v>
@@ -4389,18 +4388,18 @@
       </c>
       <c r="S26" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M26,Trigger),"--")</f>
-        <v>42895</v>
+        <v>42986</v>
       </c>
       <c r="T26" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M26,Trigger),"--")</f>
-        <v>42989</v>
+        <v>43077</v>
       </c>
       <c r="V26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W26" s="3" t="str">
-        <v>obj_0024d</v>
+        <v>obj_00298</v>
       </c>
       <c r="X26" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W26,Trigger),"")</f>
@@ -4408,7 +4407,7 @@
       </c>
       <c r="Y26" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W26,Trigger),"")</f>
-        <v>3.7675E-2</v>
+        <v>3.2774999999999999E-2</v>
       </c>
       <c r="Z26" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W26)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W26)),_xll.qlSwapRateHelperSpread($W26))</f>
@@ -4416,14 +4415,14 @@
       </c>
       <c r="AA26" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W26,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB26" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W26,Trigger),"")</f>
-        <v>49486</v>
+        <v>49584</v>
       </c>
       <c r="AC26" s="68">
-        <v>3.8561611515311511E-2</v>
+        <v>3.3562748257029276E-2</v>
       </c>
       <c r="AD26" s="158"/>
       <c r="AH26" s="156"/>
@@ -4437,7 +4436,7 @@
       </c>
       <c r="C27" s="61" t="str">
         <f>_xll.qlASXNextCode(C26,B27,Trigger)</f>
-        <v>H7</v>
+        <v>M7</v>
       </c>
       <c r="D27" s="121"/>
       <c r="E27" s="121"/>
@@ -4448,15 +4447,15 @@
       </c>
       <c r="H27" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MH7_Quote</v>
+        <v>AUDFUT3MM7_Quote</v>
       </c>
       <c r="I27" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MH7ConvAdj_Quote</v>
+        <v>AUDFUT3MM7ConvAdj_Quote</v>
       </c>
       <c r="J27" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H27,$H$15,_xll.qlASXdate(C27),G27,I27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0026f#0000</v>
+        <v>obj_002bd#0002</v>
       </c>
       <c r="K27" s="48"/>
       <c r="L27" s="9" t="str">
@@ -4465,15 +4464,15 @@
       </c>
       <c r="M27" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00271#0000</v>
+        <v>obj_002b4#0002</v>
       </c>
       <c r="N27" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M27,Trigger),"--")</f>
-        <v>AUDFUT3MU7_Quote</v>
+        <v>AUDFUT3MZ7_Quote</v>
       </c>
       <c r="O27" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M27,Trigger),"--")</f>
-        <v>97.415000000000006</v>
+        <v>97.84</v>
       </c>
       <c r="P27" s="93" t="b">
         <v>0</v>
@@ -4486,18 +4485,18 @@
       </c>
       <c r="S27" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M27,Trigger),"--")</f>
-        <v>42986</v>
+        <v>43077</v>
       </c>
       <c r="T27" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M27,Trigger),"--")</f>
-        <v>43077</v>
+        <v>43167</v>
       </c>
       <c r="V27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>Sw</v>
       </c>
       <c r="W27" s="3" t="str">
-        <v>obj_0024f</v>
+        <v>obj_00299</v>
       </c>
       <c r="X27" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W27,Trigger),"")</f>
@@ -4505,7 +4504,7 @@
       </c>
       <c r="Y27" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W27,Trigger),"")</f>
-        <v>3.8225000000000002E-2</v>
+        <v>3.2899999999999999E-2</v>
       </c>
       <c r="Z27" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W27)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W27)),_xll.qlSwapRateHelperSpread($W27))</f>
@@ -4513,14 +4512,14 @@
       </c>
       <c r="AA27" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W27,Trigger),"")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="AB27" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W27,Trigger),"")</f>
-        <v>53139</v>
+        <v>53238</v>
       </c>
       <c r="AC27" s="68">
-        <v>3.9018516569938343E-2</v>
+        <v>3.3391049364599031E-2</v>
       </c>
       <c r="AD27" s="158"/>
       <c r="AH27" s="156"/>
@@ -4534,7 +4533,7 @@
       </c>
       <c r="C28" s="61" t="str">
         <f>_xll.qlASXNextCode(C27,B28,Trigger)</f>
-        <v>M7</v>
+        <v>U7</v>
       </c>
       <c r="D28" s="121"/>
       <c r="E28" s="121"/>
@@ -4545,15 +4544,15 @@
       </c>
       <c r="H28" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MM7_Quote</v>
+        <v>AUDFUT3MU7_Quote</v>
       </c>
       <c r="I28" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MM7ConvAdj_Quote</v>
+        <v>AUDFUT3MU7ConvAdj_Quote</v>
       </c>
       <c r="J28" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H28,$H$15,_xll.qlASXdate(C28),G28,I28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00270#0000</v>
+        <v>obj_002bf#0002</v>
       </c>
       <c r="K28" s="48"/>
       <c r="L28" s="9" t="str">
@@ -4562,15 +4561,15 @@
       </c>
       <c r="M28" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00272#0000</v>
+        <v>obj_002ad#0002</v>
       </c>
       <c r="N28" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M28,Trigger),"--")</f>
-        <v>AUDFUT3MZ7_Quote</v>
+        <v>AUDFUT3MH8_Quote</v>
       </c>
       <c r="O28" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M28,Trigger),"--")</f>
-        <v>97.31</v>
+        <v>97.765000000000001</v>
       </c>
       <c r="P28" s="93" t="b">
         <v>0</v>
@@ -4583,11 +4582,11 @@
       </c>
       <c r="S28" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M28,Trigger),"--")</f>
-        <v>43077</v>
+        <v>43168</v>
       </c>
       <c r="T28" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M28,Trigger),"--")</f>
-        <v>43167</v>
+        <v>43263</v>
       </c>
       <c r="V28" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4631,7 +4630,7 @@
       </c>
       <c r="C29" s="61" t="str">
         <f>_xll.qlASXNextCode(C28,B29,Trigger)</f>
-        <v>U7</v>
+        <v>Z7</v>
       </c>
       <c r="D29" s="121"/>
       <c r="E29" s="121"/>
@@ -4642,15 +4641,15 @@
       </c>
       <c r="H29" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MU7_Quote</v>
+        <v>AUDFUT3MZ7_Quote</v>
       </c>
       <c r="I29" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MU7ConvAdj_Quote</v>
+        <v>AUDFUT3MZ7ConvAdj_Quote</v>
       </c>
       <c r="J29" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H29,$H$15,_xll.qlASXdate(C29),G29,I29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00271#0000</v>
+        <v>obj_002b4#0002</v>
       </c>
       <c r="K29" s="48"/>
       <c r="L29" s="9" t="str">
@@ -4659,15 +4658,15 @@
       </c>
       <c r="M29" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00273#0000</v>
+        <v>obj_002b7#0002</v>
       </c>
       <c r="N29" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M29,Trigger),"--")</f>
-        <v>AUDFUT3MH8_Quote</v>
+        <v>AUDFUT3MM8_Quote</v>
       </c>
       <c r="O29" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M29,Trigger),"--")</f>
-        <v>97.2</v>
+        <v>97.675000000000011</v>
       </c>
       <c r="P29" s="93" t="b">
         <v>0</v>
@@ -4680,11 +4679,11 @@
       </c>
       <c r="S29" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M29,Trigger),"--")</f>
-        <v>43168</v>
+        <v>43259</v>
       </c>
       <c r="T29" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M29,Trigger),"--")</f>
-        <v>43263</v>
+        <v>43353</v>
       </c>
       <c r="V29" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4728,7 +4727,7 @@
       </c>
       <c r="C30" s="61" t="str">
         <f>_xll.qlASXNextCode(C29,B30,Trigger)</f>
-        <v>Z7</v>
+        <v>H8</v>
       </c>
       <c r="D30" s="121"/>
       <c r="E30" s="121"/>
@@ -4739,15 +4738,15 @@
       </c>
       <c r="H30" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MZ7_Quote</v>
+        <v>AUDFUT3MH8_Quote</v>
       </c>
       <c r="I30" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MZ7ConvAdj_Quote</v>
+        <v>AUDFUT3MH8ConvAdj_Quote</v>
       </c>
       <c r="J30" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H30,$H$15,_xll.qlASXdate(C30),G30,I30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00272#0000</v>
+        <v>obj_002ad#0002</v>
       </c>
       <c r="K30" s="48"/>
       <c r="L30" s="9" t="str">
@@ -4756,15 +4755,15 @@
       </c>
       <c r="M30" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00274#0000</v>
+        <v>obj_002bc#0002</v>
       </c>
       <c r="N30" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M30,Trigger),"--")</f>
-        <v>AUDFUT3MM8_Quote</v>
+        <v>AUDFUT3MU8_Quote</v>
       </c>
       <c r="O30" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M30,Trigger),"--")</f>
-        <v>97.1</v>
+        <v>97.61</v>
       </c>
       <c r="P30" s="93" t="b">
         <v>0</v>
@@ -4777,11 +4776,11 @@
       </c>
       <c r="S30" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M30,Trigger),"--")</f>
-        <v>43259</v>
+        <v>43357</v>
       </c>
       <c r="T30" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M30,Trigger),"--")</f>
-        <v>43353</v>
+        <v>43448</v>
       </c>
       <c r="V30" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4825,7 +4824,7 @@
       </c>
       <c r="C31" s="61" t="str">
         <f>_xll.qlASXNextCode(C30,B31,Trigger)</f>
-        <v>H8</v>
+        <v>M8</v>
       </c>
       <c r="D31" s="121"/>
       <c r="E31" s="121"/>
@@ -4836,15 +4835,15 @@
       </c>
       <c r="H31" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MH8_Quote</v>
+        <v>AUDFUT3MM8_Quote</v>
       </c>
       <c r="I31" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MH8ConvAdj_Quote</v>
+        <v>AUDFUT3MM8ConvAdj_Quote</v>
       </c>
       <c r="J31" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H31,$H$15,_xll.qlASXdate(C31),G31,I31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00273#0000</v>
+        <v>obj_002b7#0002</v>
       </c>
       <c r="K31" s="48"/>
       <c r="L31" s="9" t="str">
@@ -4853,15 +4852,15 @@
       </c>
       <c r="M31" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00275#0000</v>
+        <v>obj_002b9#0002</v>
       </c>
       <c r="N31" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M31,Trigger),"--")</f>
-        <v>AUDFUT3MU8_Quote</v>
-      </c>
-      <c r="O31" s="148" t="str">
+        <v>AUDFUT3MZ8_Quote</v>
+      </c>
+      <c r="O31" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M31,Trigger),"--")</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="P31" s="93" t="b">
         <v>0</v>
@@ -4874,11 +4873,11 @@
       </c>
       <c r="S31" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M31,Trigger),"--")</f>
-        <v>43357</v>
+        <v>43448</v>
       </c>
       <c r="T31" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M31,Trigger),"--")</f>
-        <v>43448</v>
+        <v>43538</v>
       </c>
       <c r="V31" s="3" t="str">
         <f t="shared" si="3"/>
@@ -4922,7 +4921,7 @@
       </c>
       <c r="C32" s="61" t="str">
         <f>_xll.qlASXNextCode(C31,B32,Trigger)</f>
-        <v>M8</v>
+        <v>U8</v>
       </c>
       <c r="D32" s="121"/>
       <c r="E32" s="121"/>
@@ -4933,15 +4932,15 @@
       </c>
       <c r="H32" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MM8_Quote</v>
+        <v>AUDFUT3MU8_Quote</v>
       </c>
       <c r="I32" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MM8ConvAdj_Quote</v>
+        <v>AUDFUT3MU8ConvAdj_Quote</v>
       </c>
       <c r="J32" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H32,$H$15,_xll.qlASXdate(C32),G32,I32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00274#0000</v>
+        <v>obj_002bc#0002</v>
       </c>
       <c r="K32" s="48"/>
       <c r="L32" s="9" t="str">
@@ -4950,15 +4949,15 @@
       </c>
       <c r="M32" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00276#0000</v>
+        <v>obj_002ac#0002</v>
       </c>
       <c r="N32" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M32,Trigger),"--")</f>
-        <v>AUDFUT3MZ8_Quote</v>
-      </c>
-      <c r="O32" s="148" t="str">
+        <v>AUDFUT3MH9_Quote</v>
+      </c>
+      <c r="O32" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M32,Trigger),"--")</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="P32" s="93" t="b">
         <v>0</v>
@@ -4971,11 +4970,11 @@
       </c>
       <c r="S32" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M32,Trigger),"--")</f>
-        <v>43448</v>
+        <v>43532</v>
       </c>
       <c r="T32" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M32,Trigger),"--")</f>
-        <v>43538</v>
+        <v>43627</v>
       </c>
       <c r="V32" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5018,7 +5017,7 @@
       </c>
       <c r="C33" s="61" t="str">
         <f>_xll.qlASXNextCode(C32,B33,Trigger)</f>
-        <v>U8</v>
+        <v>Z8</v>
       </c>
       <c r="D33" s="121"/>
       <c r="E33" s="121"/>
@@ -5029,15 +5028,15 @@
       </c>
       <c r="H33" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MU8_Quote</v>
+        <v>AUDFUT3MZ8_Quote</v>
       </c>
       <c r="I33" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MU8ConvAdj_Quote</v>
+        <v>AUDFUT3MZ8ConvAdj_Quote</v>
       </c>
       <c r="J33" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H33,$H$15,_xll.qlASXdate(C33),G33,I33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00275#0000</v>
+        <v>obj_002b9#0002</v>
       </c>
       <c r="K33" s="48"/>
       <c r="L33" s="9" t="str">
@@ -5046,15 +5045,15 @@
       </c>
       <c r="M33" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00277#0000</v>
+        <v>obj_002b8#0002</v>
       </c>
       <c r="N33" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M33,Trigger),"--")</f>
-        <v>AUDFUT3MH9_Quote</v>
-      </c>
-      <c r="O33" s="148" t="str">
+        <v>AUDFUT3MM9_Quote</v>
+      </c>
+      <c r="O33" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M33,Trigger),"--")</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="P33" s="93" t="b">
         <v>0</v>
@@ -5067,11 +5066,11 @@
       </c>
       <c r="S33" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M33,Trigger),"--")</f>
-        <v>43532</v>
+        <v>43630</v>
       </c>
       <c r="T33" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M33,Trigger),"--")</f>
-        <v>43627</v>
+        <v>43721</v>
       </c>
       <c r="V33" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5114,7 +5113,7 @@
       </c>
       <c r="C34" s="61" t="str">
         <f>_xll.qlASXNextCode(C33,B34,Trigger)</f>
-        <v>Z8</v>
+        <v>H9</v>
       </c>
       <c r="D34" s="121"/>
       <c r="E34" s="121"/>
@@ -5125,15 +5124,15 @@
       </c>
       <c r="H34" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MZ8_Quote</v>
+        <v>AUDFUT3MH9_Quote</v>
       </c>
       <c r="I34" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MZ8ConvAdj_Quote</v>
+        <v>AUDFUT3MH9ConvAdj_Quote</v>
       </c>
       <c r="J34" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H34,$H$15,_xll.qlASXdate(C34),G34,I34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00276#0000</v>
+        <v>obj_002ac#0002</v>
       </c>
       <c r="K34" s="48"/>
       <c r="L34" s="9" t="str">
@@ -5142,15 +5141,15 @@
       </c>
       <c r="M34" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00278#0000</v>
+        <v>obj_002be#0002</v>
       </c>
       <c r="N34" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M34,Trigger),"--")</f>
-        <v>AUDFUT3MM9_Quote</v>
-      </c>
-      <c r="O34" s="148" t="str">
+        <v>AUDFUT3MU9_Quote</v>
+      </c>
+      <c r="O34" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M34,Trigger),"--")</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="P34" s="93" t="b">
         <v>0</v>
@@ -5163,11 +5162,11 @@
       </c>
       <c r="S34" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M34,Trigger),"--")</f>
-        <v>43630</v>
+        <v>43721</v>
       </c>
       <c r="T34" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M34,Trigger),"--")</f>
-        <v>43721</v>
+        <v>43812</v>
       </c>
       <c r="V34" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5210,7 +5209,7 @@
       </c>
       <c r="C35" s="61" t="str">
         <f>_xll.qlASXNextCode(C34,B35,Trigger)</f>
-        <v>H9</v>
+        <v>M9</v>
       </c>
       <c r="D35" s="121"/>
       <c r="E35" s="121"/>
@@ -5221,15 +5220,15 @@
       </c>
       <c r="H35" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MH9_Quote</v>
+        <v>AUDFUT3MM9_Quote</v>
       </c>
       <c r="I35" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MH9ConvAdj_Quote</v>
+        <v>AUDFUT3MM9ConvAdj_Quote</v>
       </c>
       <c r="J35" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H35,$H$15,_xll.qlASXdate(C35),G35,I35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00277#0000</v>
+        <v>obj_002b8#0002</v>
       </c>
       <c r="K35" s="48"/>
       <c r="L35" s="9" t="str">
@@ -5238,15 +5237,15 @@
       </c>
       <c r="M35" s="90" t="str">
         <f t="shared" si="7"/>
-        <v>obj_00279#0000</v>
+        <v>obj_002b3#0002</v>
       </c>
       <c r="N35" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M35,Trigger),"--")</f>
-        <v>AUDFUT3MU9_Quote</v>
-      </c>
-      <c r="O35" s="148" t="str">
+        <v>AUDFUT3MZ9_Quote</v>
+      </c>
+      <c r="O35" s="148">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M35,Trigger),"--")</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="P35" s="93" t="b">
         <v>0</v>
@@ -5259,11 +5258,11 @@
       </c>
       <c r="S35" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M35,Trigger),"--")</f>
-        <v>43721</v>
+        <v>43812</v>
       </c>
       <c r="T35" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M35,Trigger),"--")</f>
-        <v>43812</v>
+        <v>43903</v>
       </c>
       <c r="V35" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5306,7 +5305,7 @@
       </c>
       <c r="C36" s="61" t="str">
         <f>_xll.qlASXNextCode(C35,B36,Trigger)</f>
-        <v>M9</v>
+        <v>U9</v>
       </c>
       <c r="D36" s="121"/>
       <c r="E36" s="121"/>
@@ -5317,15 +5316,15 @@
       </c>
       <c r="H36" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MM9_Quote</v>
+        <v>AUDFUT3MU9_Quote</v>
       </c>
       <c r="I36" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MM9ConvAdj_Quote</v>
+        <v>AUDFUT3MU9ConvAdj_Quote</v>
       </c>
       <c r="J36" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H36,$H$15,_xll.qlASXdate(C36),G36,I36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00278#0000</v>
+        <v>obj_002be#0002</v>
       </c>
       <c r="K36" s="48"/>
       <c r="L36" s="10" t="str">
@@ -5334,15 +5333,15 @@
       </c>
       <c r="M36" s="91" t="str">
         <f t="shared" si="7"/>
-        <v>obj_0027a#0000</v>
+        <v>obj_002aa#0002</v>
       </c>
       <c r="N36" s="144" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M36,Trigger),"--")</f>
-        <v>AUDFUT3MZ9_Quote</v>
-      </c>
-      <c r="O36" s="149" t="str">
+        <v>AUDFUT3MH0_Quote</v>
+      </c>
+      <c r="O36" s="149">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M36,Trigger),"--")</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="P36" s="96" t="b">
         <v>0</v>
@@ -5355,11 +5354,11 @@
       </c>
       <c r="S36" s="98">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M36,Trigger),"--")</f>
-        <v>43812</v>
+        <v>43903</v>
       </c>
       <c r="T36" s="98">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M36,Trigger),"--")</f>
-        <v>43903</v>
+        <v>43997</v>
       </c>
       <c r="V36" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5402,7 +5401,7 @@
       </c>
       <c r="C37" s="61" t="str">
         <f>_xll.qlASXNextCode(C36,B37,Trigger)</f>
-        <v>U9</v>
+        <v>Z9</v>
       </c>
       <c r="D37" s="121"/>
       <c r="E37" s="121"/>
@@ -5413,15 +5412,15 @@
       </c>
       <c r="H37" s="115" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MU9_Quote</v>
+        <v>AUDFUT3MZ9_Quote</v>
       </c>
       <c r="I37" s="115" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MU9ConvAdj_Quote</v>
+        <v>AUDFUT3MZ9ConvAdj_Quote</v>
       </c>
       <c r="J37" s="62" t="str">
         <f>_xll.qlFuturesRateHelper(,H37,$H$15,_xll.qlASXdate(C37),G37,I37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00279#0000</v>
+        <v>obj_002b3#0002</v>
       </c>
       <c r="K37" s="48"/>
       <c r="L37" s="132" t="str">
@@ -5430,7 +5429,7 @@
       </c>
       <c r="M37" s="133" t="str">
         <f>IF(ISBLANK(J41),"--",J41)</f>
-        <v>obj_0024e#0000</v>
+        <v>obj_00293#0002</v>
       </c>
       <c r="N37" s="145" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M37,Trigger),"--")</f>
@@ -5438,7 +5437,7 @@
       </c>
       <c r="O37" s="135">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M37,Trigger),"--")</f>
-        <v>2.1299999999999999E-2</v>
+        <v>1.9775000000000001E-2</v>
       </c>
       <c r="P37" s="134" t="b">
         <v>0</v>
@@ -5451,11 +5450,11 @@
       </c>
       <c r="S37" s="136">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M37,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T37" s="136">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M37,Trigger),"--")</f>
-        <v>42548</v>
+        <v>42647</v>
       </c>
       <c r="V37" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5498,7 +5497,7 @@
       </c>
       <c r="C38" s="8" t="str">
         <f>_xll.qlASXNextCode(C37,B38,Trigger)</f>
-        <v>Z9</v>
+        <v>H0</v>
       </c>
       <c r="D38" s="122"/>
       <c r="E38" s="122"/>
@@ -5509,15 +5508,15 @@
       </c>
       <c r="H38" s="116" t="str">
         <f t="shared" si="9"/>
-        <v>AUDFUT3MZ9_Quote</v>
+        <v>AUDFUT3MH0_Quote</v>
       </c>
       <c r="I38" s="116" t="str">
         <f t="shared" si="10"/>
-        <v>AUDFUT3MZ9ConvAdj_Quote</v>
+        <v>AUDFUT3MH0ConvAdj_Quote</v>
       </c>
       <c r="J38" s="2" t="str">
         <f>_xll.qlFuturesRateHelper(,H38,$H$15,_xll.qlASXdate(C38),G38,I38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0027a#0000</v>
+        <v>obj_002aa#0002</v>
       </c>
       <c r="K38" s="48"/>
       <c r="L38" s="69" t="str">
@@ -5785,7 +5784,7 @@
       </c>
       <c r="J41" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(,H41,1,B41,Calendar,D41,E41,F41,G41,I41,C41,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024e#0000</v>
+        <v>obj_00293#0002</v>
       </c>
       <c r="L41" s="69" t="str">
         <f t="shared" si="11"/>
@@ -5793,7 +5792,7 @@
       </c>
       <c r="M41" s="137" t="str">
         <f t="shared" si="12"/>
-        <v>obj_00261#0000</v>
+        <v>obj_002a7#0002</v>
       </c>
       <c r="N41" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M41,Trigger),"--")</f>
@@ -5801,7 +5800,7 @@
       </c>
       <c r="O41" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M41,Trigger),"--")</f>
-        <v>2.1925E-2</v>
+        <v>1.9675000000000002E-2</v>
       </c>
       <c r="P41" s="138" t="b">
         <v>1</v>
@@ -5814,11 +5813,11 @@
       </c>
       <c r="S41" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M41,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T41" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M41,Trigger),"--")</f>
-        <v>42912</v>
+        <v>43011</v>
       </c>
       <c r="V41" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5889,7 +5888,7 @@
       </c>
       <c r="M42" s="137" t="str">
         <f t="shared" si="12"/>
-        <v>obj_00262#0000</v>
+        <v>obj_002a6#0002</v>
       </c>
       <c r="N42" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M42,Trigger),"--")</f>
@@ -5897,7 +5896,7 @@
       </c>
       <c r="O42" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M42,Trigger),"--")</f>
-        <v>2.3349999999999999E-2</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="P42" s="138" t="b">
         <v>1</v>
@@ -5910,11 +5909,11 @@
       </c>
       <c r="S42" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M42,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T42" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M42,Trigger),"--")</f>
-        <v>43277</v>
+        <v>43375</v>
       </c>
       <c r="V42" s="3" t="str">
         <f t="shared" si="3"/>
@@ -6172,7 +6171,7 @@
       </c>
       <c r="J45" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H45,1,B45,Calendar,D45,E45,F45,G45,I45,C45,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00261#0000</v>
+        <v>obj_002a7#0002</v>
       </c>
       <c r="L45" s="69" t="str">
         <f t="shared" si="11"/>
@@ -6271,7 +6270,7 @@
       </c>
       <c r="J46" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H46,1,B46,Calendar,D46,E46,F46,G46,I46,C46,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00262#0000</v>
+        <v>obj_002a6#0002</v>
       </c>
       <c r="L46" s="69" t="str">
         <f t="shared" si="11"/>
@@ -9519,7 +9518,7 @@
       </c>
       <c r="M80" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_00253#0000</v>
+        <v>obj_00296#0002</v>
       </c>
       <c r="N80" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M80,Trigger),"--")</f>
@@ -9527,7 +9526,7 @@
       </c>
       <c r="O80" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M80,Trigger),"--")</f>
-        <v>2.6050000000000004E-2</v>
+        <v>2.2675000000000001E-2</v>
       </c>
       <c r="P80" s="138" t="b">
         <v>1</v>
@@ -9540,11 +9539,11 @@
       </c>
       <c r="S80" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M80,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T80" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M80,Trigger),"--")</f>
-        <v>43642</v>
+        <v>43740</v>
       </c>
       <c r="V80" s="3" t="str">
         <f t="shared" si="15"/>
@@ -9615,7 +9614,7 @@
       </c>
       <c r="M81" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_0024b#0000</v>
+        <v>obj_00291#0002</v>
       </c>
       <c r="N81" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M81,Trigger),"--")</f>
@@ -9623,7 +9622,7 @@
       </c>
       <c r="O81" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M81,Trigger),"--")</f>
-        <v>2.7824999999999999E-2</v>
+        <v>2.3975E-2</v>
       </c>
       <c r="P81" s="138" t="b">
         <v>1</v>
@@ -9636,11 +9635,11 @@
       </c>
       <c r="S81" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M81,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T81" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M81,Trigger),"--")</f>
-        <v>44008</v>
+        <v>44106</v>
       </c>
       <c r="V81" s="3" t="str">
         <f t="shared" si="15"/>
@@ -9807,7 +9806,7 @@
       </c>
       <c r="M83" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_0024c#0000</v>
+        <v>obj_00292#0002</v>
       </c>
       <c r="N83" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M83,Trigger),"--")</f>
@@ -9815,7 +9814,7 @@
       </c>
       <c r="O83" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M83,Trigger),"--")</f>
-        <v>3.0949999999999998E-2</v>
+        <v>2.6437499999999999E-2</v>
       </c>
       <c r="P83" s="138" t="b">
         <v>1</v>
@@ -9828,11 +9827,11 @@
       </c>
       <c r="S83" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M83,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T83" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M83,Trigger),"--")</f>
-        <v>44739</v>
+        <v>44838</v>
       </c>
       <c r="V83" s="3" t="str">
         <f t="shared" si="15"/>
@@ -10090,7 +10089,7 @@
       </c>
       <c r="J86" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H86,1,B86,Calendar,D86,E86,F86,G86,I86,C86,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00253#0000</v>
+        <v>obj_00296#0002</v>
       </c>
       <c r="L86" s="69" t="str">
         <f t="shared" si="16"/>
@@ -10098,7 +10097,7 @@
       </c>
       <c r="M86" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_00252#0000</v>
+        <v>obj_00295#0002</v>
       </c>
       <c r="N86" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M86,Trigger),"--")</f>
@@ -10106,7 +10105,7 @@
       </c>
       <c r="O86" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M86,Trigger),"--")</f>
-        <v>3.4025E-2</v>
+        <v>2.9050000000000003E-2</v>
       </c>
       <c r="P86" s="138" t="b">
         <v>1</v>
@@ -10119,11 +10118,11 @@
       </c>
       <c r="S86" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M86,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T86" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M86,Trigger),"--")</f>
-        <v>45834</v>
+        <v>45932</v>
       </c>
       <c r="V86" s="3" t="str">
         <f t="shared" si="15"/>
@@ -10189,7 +10188,7 @@
       </c>
       <c r="J87" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H87,1,B87,Calendar,D87,E87,F87,G87,I87,C87,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024b#0000</v>
+        <v>obj_00291#0002</v>
       </c>
       <c r="L87" s="69" t="str">
         <f t="shared" si="16"/>
@@ -10296,7 +10295,7 @@
       </c>
       <c r="M88" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_00251#0000</v>
+        <v>obj_00294#0002</v>
       </c>
       <c r="N88" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M88,Trigger),"--")</f>
@@ -10304,7 +10303,7 @@
       </c>
       <c r="O88" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M88,Trigger),"--")</f>
-        <v>3.5425000000000005E-2</v>
+        <v>3.0250000000000003E-2</v>
       </c>
       <c r="P88" s="138" t="b">
         <v>1</v>
@@ -10317,11 +10316,11 @@
       </c>
       <c r="S88" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M88,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T88" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M88,Trigger),"--")</f>
-        <v>46566</v>
+        <v>46665</v>
       </c>
       <c r="V88" s="3" t="str">
         <f t="shared" si="15"/>
@@ -10387,7 +10386,7 @@
       </c>
       <c r="J89" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H89,1,B89,Calendar,D89,E89,F89,G89,I89,C89,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024c#0000</v>
+        <v>obj_00292#0002</v>
       </c>
       <c r="L89" s="69" t="str">
         <f t="shared" si="16"/>
@@ -10587,7 +10586,7 @@
       </c>
       <c r="M91" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_00254#0000</v>
+        <v>obj_00297#0002</v>
       </c>
       <c r="N91" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M91,Trigger),"--")</f>
@@ -10595,7 +10594,7 @@
       </c>
       <c r="O91" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M91,Trigger),"--")</f>
-        <v>3.6750000000000005E-2</v>
+        <v>3.1524999999999997E-2</v>
       </c>
       <c r="P91" s="138" t="b">
         <v>1</v>
@@ -10608,11 +10607,11 @@
       </c>
       <c r="S91" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M91,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T91" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M91,Trigger),"--")</f>
-        <v>47660</v>
+        <v>47758</v>
       </c>
       <c r="V91" s="3" t="str">
         <f t="shared" si="15"/>
@@ -10678,7 +10677,7 @@
       </c>
       <c r="J92" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H92,1,B92,Calendar,D92,E92,F92,G92,I92,C92,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00252#0000</v>
+        <v>obj_00295#0002</v>
       </c>
       <c r="L92" s="69" t="str">
         <f t="shared" si="16"/>
@@ -10873,7 +10872,7 @@
       </c>
       <c r="J94" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H94,1,B94,Calendar,D94,E94,F94,G94,I94,C94,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00251#0000</v>
+        <v>obj_00294#0002</v>
       </c>
       <c r="L94" s="69" t="str">
         <f t="shared" si="16"/>
@@ -11073,7 +11072,7 @@
       </c>
       <c r="M96" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_0024d#0000</v>
+        <v>obj_00298#0002</v>
       </c>
       <c r="N96" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M96,Trigger),"--")</f>
@@ -11081,7 +11080,7 @@
       </c>
       <c r="O96" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M96,Trigger),"--")</f>
-        <v>3.7675E-2</v>
+        <v>3.2774999999999999E-2</v>
       </c>
       <c r="P96" s="138" t="b">
         <v>1</v>
@@ -11094,11 +11093,11 @@
       </c>
       <c r="S96" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M96,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T96" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M96,Trigger),"--")</f>
-        <v>49486</v>
+        <v>49584</v>
       </c>
       <c r="V96" s="3" t="str">
         <f t="shared" si="15"/>
@@ -11164,7 +11163,7 @@
       </c>
       <c r="J97" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H97,1,B97,Calendar,D97,E97,F97,G97,I97,C97,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00254#0000</v>
+        <v>obj_00297#0002</v>
       </c>
       <c r="L97" s="69" t="str">
         <f t="shared" si="16"/>
@@ -11647,7 +11646,7 @@
       </c>
       <c r="J102" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H102,1,B102,Calendar,D102,E102,F102,G102,I102,C102,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024d#0000</v>
+        <v>obj_00298#0002</v>
       </c>
       <c r="L102" s="69" t="str">
         <f t="shared" si="16"/>
@@ -12039,7 +12038,7 @@
       </c>
       <c r="M106" s="138" t="str">
         <f t="shared" si="17"/>
-        <v>obj_0024f#0000</v>
+        <v>obj_00299#0002</v>
       </c>
       <c r="N106" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M106,Trigger),"--")</f>
@@ -12047,7 +12046,7 @@
       </c>
       <c r="O106" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M106,Trigger),"--")</f>
-        <v>3.8225000000000002E-2</v>
+        <v>3.2899999999999999E-2</v>
       </c>
       <c r="P106" s="138" t="b">
         <v>1</v>
@@ -12060,11 +12059,11 @@
       </c>
       <c r="S106" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M106,Trigger),"--")</f>
-        <v>42181</v>
+        <v>42279</v>
       </c>
       <c r="T106" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M106,Trigger),"--")</f>
-        <v>53139</v>
+        <v>53238</v>
       </c>
       <c r="V106" s="3" t="str">
         <f t="shared" si="15"/>
@@ -12547,7 +12546,7 @@
       </c>
       <c r="J112" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H112,1,B112,Calendar,D112,E112,F112,G112,I112,C112,,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0024f#0000</v>
+        <v>obj_00299#0002</v>
       </c>
       <c r="AD112" s="158"/>
     </row>

</xml_diff>